<commit_message>
Se mejora la cadena de consulta
</commit_message>
<xml_diff>
--- a/plantillas_formatos/PLANTILLA.xlsx
+++ b/plantillas_formatos/PLANTILLA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mata9585\Desktop\Dany\scripts\Python\LlenadoDeFormatos\plantillas_formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mata9585\Desktop\Dany\scripts\Python\V2\LlenadoDeFormatos\plantillas_formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7096ED4-907E-4938-B85D-891DD7A7559A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DA0B28-6AF4-45BA-A930-DCCE9359A2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -556,19 +556,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -578,23 +572,32 @@
       <alignment horizontal="center" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -627,7 +630,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -681,7 +684,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -731,7 +734,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -785,7 +788,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -835,7 +838,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -889,7 +892,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -939,7 +942,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -993,7 +996,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1043,7 +1046,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1097,7 +1100,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1147,7 +1150,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1201,7 +1204,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1251,7 +1254,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1305,7 +1308,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1355,7 +1358,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1409,7 +1412,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1459,7 +1462,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1513,7 +1516,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1563,7 +1566,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1617,7 +1620,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1667,7 +1670,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1721,7 +1724,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1771,7 +1774,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1825,7 +1828,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1875,7 +1878,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -1929,7 +1932,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1979,7 +1982,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2033,7 +2036,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2083,7 +2086,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2137,7 +2140,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2187,7 +2190,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2241,7 +2244,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2291,7 +2294,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2345,7 +2348,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2395,7 +2398,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2449,7 +2452,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>17145</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2499,7 +2502,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:colOff>1350645</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2553,7 +2556,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2921,26 +2924,27 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A4:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:G65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="7" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2966,15 +2970,15 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3242,15 +3246,15 @@
       <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3266,22 +3270,22 @@
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -3312,15 +3316,15 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:9" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3382,27 +3386,27 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -3460,15 +3464,15 @@
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
       <c r="H51" s="4"/>
       <c r="I51" s="2"/>
     </row>
@@ -3517,7 +3521,7 @@
       <c r="H55" s="17"/>
     </row>
     <row r="56" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="36" t="s">
         <v>113</v>
       </c>
       <c r="B56" s="19"/>
@@ -3529,7 +3533,7 @@
       <c r="H56" s="17"/>
     </row>
     <row r="57" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="38"/>
+      <c r="A57" s="36"/>
       <c r="B57" s="21"/>
       <c r="C57" s="5" t="s">
         <v>69</v>
@@ -3577,58 +3581,58 @@
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="37"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
       <c r="H63" s="13"/>
     </row>
     <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35"/>
+      <c r="G64" s="35"/>
       <c r="H64" s="13"/>
     </row>
     <row r="65" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
       <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,14 +3654,14 @@
       <c r="A67" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
       <c r="H67" s="4"/>
       <c r="I67" s="2"/>
     </row>
@@ -3690,15 +3694,15 @@
       <c r="H69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="32"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3712,15 +3716,15 @@
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="34"/>
       <c r="H72" s="4"/>
     </row>
     <row r="73" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3756,15 +3760,15 @@
       <c r="H75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="32" t="s">
+      <c r="A76" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="32"/>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="32"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
       <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3778,15 +3782,15 @@
       <c r="H77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B78" s="32"/>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
-      <c r="E78" s="32"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="34"/>
+      <c r="G78" s="34"/>
       <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3825,6 +3829,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="B67:G67"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A76:G76"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A46:G46"/>
@@ -3837,12 +3847,6 @@
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A45:G45"/>
     <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="B67:G67"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A76:G76"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3873,16 +3877,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
@@ -3893,14 +3897,14 @@
       <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -3909,14 +3913,14 @@
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -3925,14 +3929,14 @@
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -3941,14 +3945,14 @@
       <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -3957,14 +3961,14 @@
       <c r="B6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
@@ -3973,14 +3977,14 @@
       <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -3989,14 +3993,14 @@
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -4005,14 +4009,14 @@
       <c r="B9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -4021,14 +4025,14 @@
       <c r="B10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
@@ -4037,14 +4041,14 @@
       <c r="B11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
@@ -4053,14 +4057,14 @@
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -4069,14 +4073,14 @@
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
@@ -4085,14 +4089,14 @@
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
@@ -4101,14 +4105,14 @@
       <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
     </row>
     <row r="16" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
@@ -4117,14 +4121,14 @@
       <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
     </row>
     <row r="17" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -4133,14 +4137,14 @@
       <c r="B17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
     </row>
     <row r="18" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
@@ -4149,14 +4153,14 @@
       <c r="B18" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
     </row>
     <row r="19" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
@@ -4165,14 +4169,14 @@
       <c r="B19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" spans="1:8" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
@@ -4181,14 +4185,14 @@
       <c r="B20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
@@ -4197,14 +4201,14 @@
       <c r="B21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
@@ -4213,14 +4217,14 @@
       <c r="B22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -4229,14 +4233,14 @@
       <c r="B23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
@@ -4245,14 +4249,14 @@
       <c r="B24" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
@@ -4261,14 +4265,14 @@
       <c r="B25" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
@@ -4277,14 +4281,14 @@
       <c r="B26" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
@@ -4293,14 +4297,14 @@
       <c r="B27" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
     </row>
     <row r="28" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -4309,29 +4313,17 @@
       <c r="B28" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="C22:H22"/>
@@ -4348,6 +4340,18 @@
     <mergeCell ref="C9:H9"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C24:H24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0" footer="0"/>

</xml_diff>